<commit_message>
Implemented Excel for Univ Generation
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE07FC82-D4BA-47A0-80A7-C9F00CB2FD1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A6DD4-60E1-4BCF-AC21-6EDEE639B093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
-    <sheet name="Promotions" sheetId="3" r:id="rId2"/>
-    <sheet name="Subjects" sheetId="2" r:id="rId3"/>
+    <sheet name="Timeslots" sheetId="6" r:id="rId2"/>
+    <sheet name="Promotions" sheetId="3" r:id="rId3"/>
+    <sheet name="Subjects" sheetId="2" r:id="rId4"/>
+    <sheet name="Teachers" sheetId="4" r:id="rId5"/>
+    <sheet name="Rooms" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -86,6 +89,171 @@
   </si>
   <si>
     <t>Hours</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>UNI011</t>
+  </si>
+  <si>
+    <t>UNI023</t>
+  </si>
+  <si>
+    <t>UNI021</t>
+  </si>
+  <si>
+    <t>UNI022</t>
+  </si>
+  <si>
+    <t>UNI012</t>
+  </si>
+  <si>
+    <t>UNI013</t>
+  </si>
+  <si>
+    <t>0c0fcc</t>
+  </si>
+  <si>
+    <t>9008d4</t>
+  </si>
+  <si>
+    <t>05e6de</t>
+  </si>
+  <si>
+    <t>0a0ca3</t>
+  </si>
+  <si>
+    <t>55047d</t>
+  </si>
+  <si>
+    <t>07b3ac</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Idt</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>L101</t>
+  </si>
+  <si>
+    <t>L102</t>
+  </si>
+  <si>
+    <t>L103</t>
+  </si>
+  <si>
+    <t>L104</t>
+  </si>
+  <si>
+    <t>L105</t>
+  </si>
+  <si>
+    <t>AmphiC</t>
+  </si>
+  <si>
+    <t>Amphitheatre</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Start day</t>
+  </si>
+  <si>
+    <t>Start month</t>
+  </si>
+  <si>
+    <t>Start year</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>StartH</t>
+  </si>
+  <si>
+    <t>StartMin</t>
+  </si>
+  <si>
+    <t>EndH</t>
+  </si>
+  <si>
+    <t>EndMin</t>
+  </si>
+  <si>
+    <t>Subjects (séparés d'un '-')</t>
+  </si>
+  <si>
+    <t>Henri</t>
+  </si>
+  <si>
+    <t>Barbeau</t>
+  </si>
+  <si>
+    <t>Timothé</t>
+  </si>
+  <si>
+    <t>Solé</t>
+  </si>
+  <si>
+    <t>Renaud</t>
+  </si>
+  <si>
+    <t>Cerfbeer</t>
+  </si>
+  <si>
+    <t>Christiane</t>
+  </si>
+  <si>
+    <t>Brunelle</t>
+  </si>
+  <si>
+    <t>Constantin</t>
+  </si>
+  <si>
+    <t>Poussin</t>
+  </si>
+  <si>
+    <t>Maurice</t>
+  </si>
+  <si>
+    <t>Vannier</t>
+  </si>
+  <si>
+    <t>Napoléon</t>
+  </si>
+  <si>
+    <t>Matthieu</t>
+  </si>
+  <si>
+    <t>Josette</t>
+  </si>
+  <si>
+    <t>Paquin</t>
+  </si>
+  <si>
+    <t>UNI011-UNI021</t>
+  </si>
+  <si>
+    <t>UNI012-UNI022</t>
+  </si>
+  <si>
+    <t>UNI013-UNI023</t>
   </si>
 </sst>
 </file>
@@ -457,10 +625,525 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB5D4C-C765-4C0B-97C4-EF4AAF1E2B40}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4ED29B7-73F5-491F-B3D4-024DDAB798D5}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215C1F2-9091-436A-A149-7A9EF9562B8F}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="70" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EF849C-ECD7-4B59-8B07-8EA41506542A}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13FFBB7-0715-45C0-A6D5-76680980035E}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,170 +1153,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215C1F2-9091-436A-A149-7A9EF9562B8F}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="70" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>5</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed noRoomOverlap and noTeacherOverlap
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9A6DD4-60E1-4BCF-AC21-6EDEE639B093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D74DF9-54B5-412D-AC07-8C6C77FBDD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-32535" yWindow="-4455" windowWidth="23880" windowHeight="15285" activeTab="5" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>UNI013-UNI023</t>
+  </si>
+  <si>
+    <t>Achille</t>
+  </si>
+  <si>
+    <t>Cochet</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>D'Aboville</t>
   </si>
 </sst>
 </file>
@@ -817,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -996,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EF849C-ECD7-4B59-8B07-8EA41506542A}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1068,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1082,13 +1094,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1096,13 +1108,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1110,13 +1122,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1124,12 +1136,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>66</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>67</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1142,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13FFBB7-0715-45C0-A6D5-76680980035E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v0.0.1 - User friendliness
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D74DF9-54B5-412D-AC07-8C6C77FBDD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77BF61F-D11E-4A9A-AC6A-00CD621E2C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32535" yWindow="-4455" windowWidth="23880" windowHeight="15285" activeTab="5" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -58,12 +58,6 @@
     <t>TDA</t>
   </si>
   <si>
-    <t>TDB</t>
-  </si>
-  <si>
-    <t>TDC</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -112,24 +106,6 @@
     <t>UNI013</t>
   </si>
   <si>
-    <t>0c0fcc</t>
-  </si>
-  <si>
-    <t>9008d4</t>
-  </si>
-  <si>
-    <t>05e6de</t>
-  </si>
-  <si>
-    <t>0a0ca3</t>
-  </si>
-  <si>
-    <t>55047d</t>
-  </si>
-  <si>
-    <t>07b3ac</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -157,12 +133,6 @@
     <t>L105</t>
   </si>
   <si>
-    <t>AmphiC</t>
-  </si>
-  <si>
-    <t>Amphitheatre</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -247,15 +217,6 @@
     <t>Paquin</t>
   </si>
   <si>
-    <t>UNI011-UNI021</t>
-  </si>
-  <si>
-    <t>UNI012-UNI022</t>
-  </si>
-  <si>
-    <t>UNI013-UNI023</t>
-  </si>
-  <si>
     <t>Achille</t>
   </si>
   <si>
@@ -266,6 +227,162 @@
   </si>
   <si>
     <t>D'Aboville</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>UNI014</t>
+  </si>
+  <si>
+    <t>Basic Chemistry</t>
+  </si>
+  <si>
+    <t>UNI015</t>
+  </si>
+  <si>
+    <t>Basic Biology</t>
+  </si>
+  <si>
+    <t>UNI016</t>
+  </si>
+  <si>
+    <t>Basic Engineering</t>
+  </si>
+  <si>
+    <t>UNI024</t>
+  </si>
+  <si>
+    <t>Advanced Chemistry</t>
+  </si>
+  <si>
+    <t>UNI025</t>
+  </si>
+  <si>
+    <t>Advanced Biology</t>
+  </si>
+  <si>
+    <t>UNI026</t>
+  </si>
+  <si>
+    <t>Advanced Engineering</t>
+  </si>
+  <si>
+    <t>UNI031</t>
+  </si>
+  <si>
+    <t>Applied Mathematics</t>
+  </si>
+  <si>
+    <t>UNI032</t>
+  </si>
+  <si>
+    <t>Quantum Mechanics</t>
+  </si>
+  <si>
+    <t>UNI033</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>UNI034</t>
+  </si>
+  <si>
+    <t>Organic Chemistry</t>
+  </si>
+  <si>
+    <t>UNI035</t>
+  </si>
+  <si>
+    <t>Genetics</t>
+  </si>
+  <si>
+    <t>UNI036</t>
+  </si>
+  <si>
+    <t>Mechanical Systems</t>
+  </si>
+  <si>
+    <t>FF33A8</t>
+  </si>
+  <si>
+    <t>33FF57</t>
+  </si>
+  <si>
+    <t>33A8FF</t>
+  </si>
+  <si>
+    <t>FFD700</t>
+  </si>
+  <si>
+    <t>FF8C00</t>
+  </si>
+  <si>
+    <t>DC143C</t>
+  </si>
+  <si>
+    <t>8A2BE2</t>
+  </si>
+  <si>
+    <t>00FA9A</t>
+  </si>
+  <si>
+    <t>1E90FF</t>
+  </si>
+  <si>
+    <t>FF4500</t>
+  </si>
+  <si>
+    <t>FF5733</t>
+  </si>
+  <si>
+    <t>UNI011-UNI021-UNI031-UNI041-UNI051</t>
+  </si>
+  <si>
+    <t>UNI012-UNI022-UNI032-UNI042-UNI052</t>
+  </si>
+  <si>
+    <t>UNI013-UNI023-UNI033-UNI043-UNI053</t>
+  </si>
+  <si>
+    <t>UNI014-UNI024-UNI034-UNI044-UNI054</t>
+  </si>
+  <si>
+    <t>UNI015-UNI025-UNI035-UNI045-UNI055</t>
+  </si>
+  <si>
+    <t>UNI016-UNI026-UNI036-UNI046-UNI056</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>L106</t>
+  </si>
+  <si>
+    <t>FF1493</t>
+  </si>
+  <si>
+    <t>9932CC</t>
+  </si>
+  <si>
+    <t>00CED1</t>
+  </si>
+  <si>
+    <t>4682B4</t>
+  </si>
+  <si>
+    <t>FFA500</t>
   </si>
 </sst>
 </file>
@@ -301,8 +418,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,17 +764,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +787,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -671,7 +795,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -679,7 +803,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>2025</v>
@@ -687,10 +811,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -703,23 +827,23 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -827,41 +951,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -871,135 +988,376 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215C1F2-9091-436A-A149-7A9EF9562B8F}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I8:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E14" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="1">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="1">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
+      <c r="E18" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="1">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1008,29 +1366,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EF849C-ECD7-4B59-8B07-8EA41506542A}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1038,13 +1396,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1052,13 +1410,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1066,13 +1424,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1080,13 +1438,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1094,13 +1452,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1108,13 +1466,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>69</v>
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1122,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1136,13 +1494,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1150,13 +1508,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1164,14 +1522,45 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>70</v>
-      </c>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1182,8 +1571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E13FFBB7-0715-45C0-A6D5-76680980035E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,55 +1582,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.1.2 - Optimized noRoomOverlap
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77BF61F-D11E-4A9A-AC6A-00CD621E2C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210D189-F18A-4CBB-AD09-D72398A57B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I8:I9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>87</v>
@@ -1062,7 +1062,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>88</v>
@@ -1079,7 +1079,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>89</v>
@@ -1096,7 +1096,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>90</v>
@@ -1130,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>92</v>
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>95</v>
@@ -1198,7 +1198,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>90</v>
@@ -1249,7 +1249,7 @@
         <v>62</v>
       </c>
       <c r="D15" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>110</v>
@@ -1266,7 +1266,7 @@
         <v>62</v>
       </c>
       <c r="D16" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>111</v>
@@ -1300,7 +1300,7 @@
         <v>62</v>
       </c>
       <c r="D18" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
v0.1.4 - Fixed bad optim
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210D189-F18A-4CBB-AD09-D72398A57B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80761B6-171F-433C-BA2A-D85D2A6DF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB5D4C-C765-4C0B-97C4-EF4AAF1E2B40}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B215C1F2-9091-436A-A149-7A9EF9562B8F}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1572,7 +1572,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
v0.1.4b - Added the CPU and RAM tracking
</commit_message>
<xml_diff>
--- a/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
+++ b/GoodwingTimetabler/UniversityInstance/UniversityGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbonn\Desktop\ESILV\A4\PI2\GitHub_PI2\GoodwingTimetabler\UniversityInstance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80761B6-171F-433C-BA2A-D85D2A6DF2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF22379-5F18-496A-8362-5936CB53772F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{B72B09E8-A954-412D-973D-4D6537A5C659}"/>
   </bookViews>
   <sheets>
     <sheet name="University" sheetId="1" r:id="rId1"/>
@@ -763,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42AB5D4C-C765-4C0B-97C4-EF4AAF1E2B40}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E3E0C2-CBFD-441F-AB28-E61B30CAF7BA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>